<commit_message>
UPDATE: modificacion de los excel y las importaciones
</commit_message>
<xml_diff>
--- a/excel/Alumnos.xlsx
+++ b/excel/Alumnos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Incidencias_EVG\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php_isa\Incidencias_EVG\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,9 +50,6 @@
     <t>Telefono</t>
   </si>
   <si>
-    <t>Bonilla Pizarro, Juan Francisco</t>
-  </si>
-  <si>
     <t>Carmona González, Pablo</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Bonilla Pizarro, Juan Francisca</t>
   </si>
 </sst>
 </file>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,13 +664,13 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6">
         <v>634230211</v>
@@ -681,13 +681,13 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6">
         <v>634230211</v>
@@ -698,30 +698,30 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6">
         <v>634230211</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="6">
         <v>634230211</v>
@@ -732,13 +732,13 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6">
         <v>634230211</v>
@@ -749,13 +749,13 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="6">
         <v>634230211</v>
@@ -766,13 +766,13 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6">
         <v>634230211</v>
@@ -783,13 +783,13 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="6">
         <v>634230211</v>
@@ -800,13 +800,13 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="6">
         <v>634230211</v>
@@ -817,13 +817,13 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="6">
         <v>634230211</v>
@@ -834,13 +834,13 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="6">
         <v>634230211</v>
@@ -852,13 +852,13 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="6">
         <v>634230211</v>
@@ -869,13 +869,13 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="6">
         <v>634230211</v>
@@ -886,30 +886,30 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="6">
         <v>634230211</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="6">
         <v>634230211</v>
@@ -926,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="6">
         <v>634230211</v>
@@ -937,13 +937,13 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="6">
         <v>634230211</v>
@@ -954,13 +954,13 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="6">
         <v>634230211</v>
@@ -971,13 +971,13 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="6">
         <v>634230211</v>
@@ -988,13 +988,13 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="6">
         <v>634230211</v>
@@ -1005,13 +1005,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="6">
         <v>634230211</v>
@@ -1022,13 +1022,13 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="6">
         <v>634230211</v>
@@ -1039,13 +1039,13 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="6">
         <v>634230211</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" s="6">
         <v>634230211</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="6">
         <v>634230211</v>

</xml_diff>

<commit_message>
UPDATE: SCRIPT Y MAS COSILLAS JEJE
</commit_message>
<xml_diff>
--- a/excel/Alumnos.xlsx
+++ b/excel/Alumnos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php_isa\Incidencias_EVG\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Incidencias_EVG\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>N.I.A.</t>
   </si>
@@ -198,6 +198,18 @@
   </si>
   <si>
     <t>Bonilla Pizarro, Juan Francisca</t>
+  </si>
+  <si>
+    <t>1ESOA</t>
+  </si>
+  <si>
+    <t>BC1C</t>
+  </si>
+  <si>
+    <t>BC1B</t>
+  </si>
+  <si>
+    <t>2ESOC</t>
   </si>
 </sst>
 </file>
@@ -640,7 +652,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B10" sqref="B10:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +815,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>39</v>
@@ -820,7 +832,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>40</v>
@@ -837,7 +849,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>41</v>
@@ -855,7 +867,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>42</v>
@@ -872,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>43</v>
@@ -889,7 +901,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>44</v>
@@ -906,7 +918,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>45</v>
@@ -923,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>46</v>
@@ -940,7 +952,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>47</v>
@@ -957,7 +969,7 @@
         <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>48</v>
@@ -974,7 +986,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>49</v>
@@ -991,7 +1003,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>50</v>
@@ -1008,7 +1020,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>51</v>
@@ -1025,7 +1037,7 @@
         <v>27</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>52</v>
@@ -1042,7 +1054,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>53</v>
@@ -1059,7 +1071,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>54</v>
@@ -1076,7 +1088,7 @@
         <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>55</v>

</xml_diff>